<commit_message>
revising 2023 program names to match year tracking convention
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_market_garden_data_2023_clean.xlsx
+++ b/analytics/modified_data/tbf_market_garden_data_2023_clean.xlsx
@@ -16948,10 +16948,10 @@
         <v>147</v>
       </c>
       <c r="BS27" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="BT27" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="BU27" t="s">
         <v>153</v>
@@ -17510,10 +17510,10 @@
         <v>147</v>
       </c>
       <c r="BS28" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="BT28" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="BU28" t="s">
         <v>153</v>

</xml_diff>